<commit_message>
old gerber files removed and BOM updated
</commit_message>
<xml_diff>
--- a/hardware/PCB/SingleBoard/BOM_v0.2.xlsx
+++ b/hardware/PCB/SingleBoard/BOM_v0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\hardware\PCB\SingleBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A9CE37-98D7-402D-BAE2-995826BDD521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B87506-A23E-40E7-9BDA-6EEE17C87689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41280" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +678,7 @@
         <v>3.5590000000000002</v>
       </c>
       <c r="G2" s="2">
-        <f>F2*D2</f>
+        <f t="shared" ref="G2:G8" si="0">F2*D2</f>
         <v>3.5590000000000002</v>
       </c>
     </row>
@@ -702,7 +702,7 @@
         <v>39.44</v>
       </c>
       <c r="G3" s="2">
-        <f>F3*D3</f>
+        <f t="shared" si="0"/>
         <v>39.44</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -726,7 +726,7 @@
         <v>2.15</v>
       </c>
       <c r="G4" s="2">
-        <f>F4*D4</f>
+        <f t="shared" si="0"/>
         <v>4.3</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -750,7 +750,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="G5" s="2">
-        <f>F5*D5</f>
+        <f t="shared" si="0"/>
         <v>0.112</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -778,7 +778,7 @@
         <v>0.186</v>
       </c>
       <c r="G6" s="2">
-        <f>F6*D6</f>
+        <f t="shared" si="0"/>
         <v>0.92999999999999994</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -803,7 +803,7 @@
         <v>0.121</v>
       </c>
       <c r="G7" s="2">
-        <f>F7*D7</f>
+        <f t="shared" si="0"/>
         <v>0.121</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -828,7 +828,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="G8" s="2">
-        <f>F8*D8</f>
+        <f t="shared" si="0"/>
         <v>0.14199999999999999</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -853,7 +853,7 @@
         <v>0.72799999999999998</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ref="G9:G11" si="0">F9*D9</f>
+        <f t="shared" ref="G9:G11" si="1">F9*D9</f>
         <v>0.72799999999999998</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -878,7 +878,7 @@
         <v>0.51200000000000001</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.51200000000000001</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -904,7 +904,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19800000000000001</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -925,7 +925,7 @@
         <v>1.93</v>
       </c>
       <c r="G12" s="2">
-        <f>F12*D12</f>
+        <f t="shared" ref="G12:G20" si="2">F12*D12</f>
         <v>3.86</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -943,7 +943,7 @@
         <v>7.06</v>
       </c>
       <c r="G13" s="2">
-        <f>F13*D13</f>
+        <f t="shared" si="2"/>
         <v>7.06</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -961,7 +961,7 @@
         <v>6.65</v>
       </c>
       <c r="G14" s="2">
-        <f>F14*D14</f>
+        <f t="shared" si="2"/>
         <v>6.65</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -979,7 +979,7 @@
         <v>21.52</v>
       </c>
       <c r="G15" s="2">
-        <f>F15*D15</f>
+        <f t="shared" si="2"/>
         <v>21.52</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -997,7 +997,7 @@
         <v>15.23</v>
       </c>
       <c r="G16" s="2">
-        <f>F16*D16</f>
+        <f t="shared" si="2"/>
         <v>15.23</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -1015,7 +1015,7 @@
         <v>8.1</v>
       </c>
       <c r="G17" s="2">
-        <f>F17*D17</f>
+        <f t="shared" si="2"/>
         <v>8.1</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -1033,7 +1033,7 @@
         <v>18.5</v>
       </c>
       <c r="G18" s="2">
-        <f>F18*D18</f>
+        <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -1052,7 +1052,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="G19" s="2">
-        <f>F19*D19</f>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -1073,7 +1073,7 @@
         <v>18.32</v>
       </c>
       <c r="G20" s="2">
-        <f>F20*D20</f>
+        <f t="shared" si="2"/>
         <v>36.64</v>
       </c>
       <c r="H20" s="1" t="s">

</xml_diff>